<commit_message>
Add SQF-RNN results and evalutation
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavel\Documents\GEFCom14-S-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD034BC5-B782-4173-9431-B874AACBD6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5823824-C99A-47E1-B6AD-5AF38D66CD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59190" yWindow="1395" windowWidth="21990" windowHeight="18930" tabRatio="931" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="2100" windowWidth="21345" windowHeight="18930" tabRatio="931" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary-1" sheetId="32" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="345">
   <si>
     <t>Load</t>
   </si>
@@ -1062,6 +1062,24 @@
   </si>
   <si>
     <t>ensemble_count=7, epochs=7</t>
+  </si>
+  <si>
+    <t>nnqf with TP</t>
+  </si>
+  <si>
+    <t>sqf-rnn with TP, TCC</t>
+  </si>
+  <si>
+    <t>sqf-rnn with TP</t>
+  </si>
+  <si>
+    <t>nnqf with TP, TCC</t>
+  </si>
+  <si>
+    <t>nnqf with TCC</t>
+  </si>
+  <si>
+    <t>task</t>
   </si>
 </sst>
 </file>
@@ -9290,10 +9308,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10203,55 +10221,146 @@
       <c r="M24">
         <v>1.949E-2</v>
       </c>
-      <c r="O24" t="s">
+    </row>
+    <row r="25" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="L25" s="14">
+        <v>1.6650000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B26" s="14">
+        <v>2.3130000000000001E-2</v>
+      </c>
+      <c r="C26" s="14">
+        <v>2.921E-2</v>
+      </c>
+      <c r="D26" s="14">
+        <v>2.4910000000000002E-2</v>
+      </c>
+      <c r="E26" s="14">
+        <v>2.445E-2</v>
+      </c>
+      <c r="F26" s="14">
+        <v>2.0549999999999999E-2</v>
+      </c>
+      <c r="G26" s="14">
+        <v>2.0570000000000001E-2</v>
+      </c>
+      <c r="H26" s="33">
+        <v>1.925E-2</v>
+      </c>
+      <c r="I26" s="14">
+        <v>1.942E-2</v>
+      </c>
+      <c r="J26" s="14">
+        <v>2.1649999999999999E-2</v>
+      </c>
+      <c r="K26" s="14">
+        <v>2.231E-2</v>
+      </c>
+      <c r="L26" s="14">
+        <v>1.2070000000000001E-2</v>
+      </c>
+      <c r="M26" s="14">
+        <v>1.916E-2</v>
+      </c>
+      <c r="O26" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="F27">
+        <v>3.3480000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="F28" s="33">
+        <v>3.3759999999999998E-2</v>
+      </c>
+      <c r="H28" s="14">
+        <v>2.9510000000000002E-2</v>
+      </c>
+      <c r="L28" s="14">
+        <v>2.1899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="F29" s="14">
+        <v>3.363E-2</v>
+      </c>
+      <c r="L29" s="14">
+        <v>2.2800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="F30" s="14">
+        <v>3.3180000000000001E-2</v>
+      </c>
+      <c r="L30" s="14">
+        <v>2.2790000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B28">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B33">
         <v>4</v>
       </c>
-      <c r="C28">
+      <c r="C33">
         <v>5</v>
       </c>
-      <c r="D28">
+      <c r="D33">
         <v>6</v>
       </c>
-      <c r="E28">
+      <c r="E33">
         <v>7</v>
       </c>
-      <c r="F28">
+      <c r="F33">
         <v>8</v>
       </c>
-      <c r="G28">
+      <c r="G33">
         <v>9</v>
       </c>
-      <c r="H28">
+      <c r="H33">
         <v>10</v>
       </c>
-      <c r="I28">
+      <c r="I33">
         <v>11</v>
       </c>
-      <c r="J28">
+      <c r="J33">
         <v>12</v>
       </c>
-      <c r="K28">
+      <c r="K33">
         <v>13</v>
       </c>
-      <c r="L28">
+      <c r="L33">
         <v>14</v>
       </c>
-      <c r="M28">
+      <c r="M33">
         <v>15</v>
       </c>
     </row>
@@ -11508,10 +11617,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A24" sqref="A24:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12477,7 +12586,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B25" s="42">
         <f>'S-score-0'!B25</f>
@@ -12521,7 +12630,7 @@
       </c>
       <c r="L25" s="42">
         <f>'S-score-0'!L25</f>
-        <v>0</v>
+        <v>1.6650000000000002E-2</v>
       </c>
       <c r="M25" s="42">
         <f>'S-score-0'!M25</f>
@@ -12530,54 +12639,319 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B26" s="42">
         <f>'S-score-0'!B26</f>
-        <v>0</v>
+        <v>2.3130000000000001E-2</v>
       </c>
       <c r="C26" s="42">
         <f>'S-score-0'!C26</f>
-        <v>0</v>
+        <v>2.921E-2</v>
       </c>
       <c r="D26" s="42">
         <f>'S-score-0'!D26</f>
-        <v>0</v>
+        <v>2.4910000000000002E-2</v>
       </c>
       <c r="E26" s="42">
         <f>'S-score-0'!E26</f>
-        <v>0</v>
+        <v>2.445E-2</v>
       </c>
       <c r="F26" s="42">
         <f>'S-score-0'!F26</f>
-        <v>0</v>
+        <v>2.0549999999999999E-2</v>
       </c>
       <c r="G26" s="42">
         <f>'S-score-0'!G26</f>
-        <v>0</v>
+        <v>2.0570000000000001E-2</v>
       </c>
       <c r="H26" s="42">
         <f>'S-score-0'!H26</f>
-        <v>0</v>
+        <v>1.925E-2</v>
       </c>
       <c r="I26" s="42">
         <f>'S-score-0'!I26</f>
-        <v>0</v>
+        <v>1.942E-2</v>
       </c>
       <c r="J26" s="42">
         <f>'S-score-0'!J26</f>
-        <v>0</v>
+        <v>2.1649999999999999E-2</v>
       </c>
       <c r="K26" s="42">
         <f>'S-score-0'!K26</f>
-        <v>0</v>
+        <v>2.231E-2</v>
       </c>
       <c r="L26" s="42">
         <f>'S-score-0'!L26</f>
-        <v>0</v>
+        <v>1.2070000000000001E-2</v>
       </c>
       <c r="M26" s="42">
         <f>'S-score-0'!M26</f>
+        <v>1.916E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B27" s="42">
+        <f>'S-score-0'!B27</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="42">
+        <f>'S-score-0'!C27</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="42">
+        <f>'S-score-0'!D27</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="42">
+        <f>'S-score-0'!E27</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="42">
+        <f>'S-score-0'!F27</f>
+        <v>3.3480000000000003E-2</v>
+      </c>
+      <c r="G27" s="42">
+        <f>'S-score-0'!G27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="42">
+        <f>'S-score-0'!H27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="42">
+        <f>'S-score-0'!I27</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="42">
+        <f>'S-score-0'!J27</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="42">
+        <f>'S-score-0'!K27</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="42">
+        <f>'S-score-0'!L27</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="42">
+        <f>'S-score-0'!M27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B28" s="42">
+        <f>'S-score-0'!B28</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="42">
+        <f>'S-score-0'!C28</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="42">
+        <f>'S-score-0'!D28</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="42">
+        <f>'S-score-0'!E28</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="42">
+        <f>'S-score-0'!F28</f>
+        <v>3.3759999999999998E-2</v>
+      </c>
+      <c r="G28" s="42">
+        <f>'S-score-0'!G28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="42">
+        <f>'S-score-0'!H28</f>
+        <v>2.9510000000000002E-2</v>
+      </c>
+      <c r="I28" s="42">
+        <f>'S-score-0'!I28</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="42">
+        <f>'S-score-0'!J28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="42">
+        <f>'S-score-0'!K28</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="42">
+        <f>'S-score-0'!L28</f>
+        <v>2.1899999999999999E-2</v>
+      </c>
+      <c r="M28" s="42">
+        <f>'S-score-0'!M28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B29" s="42">
+        <f>'S-score-0'!B29</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="42">
+        <f>'S-score-0'!C29</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="42">
+        <f>'S-score-0'!D29</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="42">
+        <f>'S-score-0'!E29</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="42">
+        <f>'S-score-0'!F29</f>
+        <v>3.363E-2</v>
+      </c>
+      <c r="G29" s="42">
+        <f>'S-score-0'!G29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="42">
+        <f>'S-score-0'!H29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="42">
+        <f>'S-score-0'!I29</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="42">
+        <f>'S-score-0'!J29</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="42">
+        <f>'S-score-0'!K29</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="42">
+        <f>'S-score-0'!L29</f>
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="M29" s="42">
+        <f>'S-score-0'!M29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B30" s="42">
+        <f>'S-score-0'!B30</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="42">
+        <f>'S-score-0'!C30</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="42">
+        <f>'S-score-0'!D30</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="42">
+        <f>'S-score-0'!E30</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="42">
+        <f>'S-score-0'!F30</f>
+        <v>3.3180000000000001E-2</v>
+      </c>
+      <c r="G30" s="42">
+        <f>'S-score-0'!G30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="42">
+        <f>'S-score-0'!H30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="42">
+        <f>'S-score-0'!I30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="42">
+        <f>'S-score-0'!J30</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="42">
+        <f>'S-score-0'!K30</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="42">
+        <f>'S-score-0'!L30</f>
+        <v>2.2790000000000001E-2</v>
+      </c>
+      <c r="M30" s="42">
+        <f>'S-score-0'!M30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" s="42">
+        <f>'S-score-0'!B31</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="42">
+        <f>'S-score-0'!C31</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="42">
+        <f>'S-score-0'!D31</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="42">
+        <f>'S-score-0'!E31</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="42">
+        <f>'S-score-0'!F31</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="42">
+        <f>'S-score-0'!G31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="42">
+        <f>'S-score-0'!H31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="42">
+        <f>'S-score-0'!I31</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="42">
+        <f>'S-score-0'!J31</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="42">
+        <f>'S-score-0'!K31</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="42">
+        <f>'S-score-0'!L31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="42">
+        <f>'S-score-0'!M31</f>
         <v>0</v>
       </c>
     </row>
@@ -12591,10 +12965,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13987,10 +14361,14 @@
         <f>SUMPRODUCT(B$1:M$1,B24:M24)/SUM(B$1:M$1)</f>
         <v>0.35895576640249222</v>
       </c>
+      <c r="O24" s="14">
+        <f>RANK(N24,(N$2:N$22,N24))</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B25" s="14">
         <f>1-'S-score-2'!B25/'S-score-2'!B$4</f>
@@ -14034,71 +14412,384 @@
       </c>
       <c r="L25" s="14">
         <f>1-'S-score-2'!L25/'S-score-2'!L$4</f>
-        <v>1</v>
+        <v>0.47919924929621516</v>
       </c>
       <c r="M25" s="14">
         <f>1-'S-score-2'!M25/'S-score-2'!M$4</f>
         <v>1</v>
       </c>
       <c r="N25" s="43">
-        <f t="shared" ref="N25:N26" si="2">SUMPRODUCT(B$1:M$1,B25:M25)/SUM(B$1:M$1)</f>
+        <f t="shared" ref="N25:N31" si="2">SUMPRODUCT(B$1:M$1,B25:M25)/SUM(B$1:M$1)</f>
+        <v>0.92655374028536364</v>
+      </c>
+      <c r="O25" s="14">
+        <f>RANK(N25,(N$2:N$22,N25))</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B26" s="14">
         <f>1-'S-score-2'!B26/'S-score-2'!B$4</f>
-        <v>1</v>
+        <v>0.30120845921450146</v>
       </c>
       <c r="C26" s="14">
         <f>1-'S-score-2'!C26/'S-score-2'!C$4</f>
-        <v>1</v>
+        <v>0.24735892811131144</v>
       </c>
       <c r="D26" s="14">
         <f>1-'S-score-2'!D26/'S-score-2'!D$4</f>
-        <v>1</v>
+        <v>0.30632135895293777</v>
       </c>
       <c r="E26" s="14">
         <f>1-'S-score-2'!E26/'S-score-2'!E$4</f>
-        <v>1</v>
+        <v>0.32196339434276211</v>
       </c>
       <c r="F26" s="14">
         <f>1-'S-score-2'!F26/'S-score-2'!F$4</f>
-        <v>1</v>
+        <v>0.57080200501253131</v>
       </c>
       <c r="G26" s="14">
         <f>1-'S-score-2'!G26/'S-score-2'!G$4</f>
-        <v>1</v>
+        <v>0.42364808069487248</v>
       </c>
       <c r="H26" s="14">
         <f>1-'S-score-2'!H26/'S-score-2'!H$4</f>
-        <v>1</v>
+        <v>0.54297245963912633</v>
       </c>
       <c r="I26" s="14">
         <f>1-'S-score-2'!I26/'S-score-2'!I$4</f>
-        <v>1</v>
+        <v>0.5134051616136307</v>
       </c>
       <c r="J26" s="14">
         <f>1-'S-score-2'!J26/'S-score-2'!J$4</f>
-        <v>1</v>
+        <v>0.5024132383360147</v>
       </c>
       <c r="K26" s="14">
         <f>1-'S-score-2'!K26/'S-score-2'!K$4</f>
-        <v>1</v>
+        <v>0.40743691899070389</v>
       </c>
       <c r="L26" s="14">
         <f>1-'S-score-2'!L26/'S-score-2'!L$4</f>
-        <v>1</v>
+        <v>0.62245855489521418</v>
       </c>
       <c r="M26" s="14">
         <f>1-'S-score-2'!M26/'S-score-2'!M$4</f>
-        <v>1</v>
+        <v>0.32748332748332754</v>
       </c>
       <c r="N26" s="43">
         <f t="shared" si="2"/>
+        <v>0.4574310686905162</v>
+      </c>
+      <c r="O26" s="14">
+        <f>RANK(N26,(N$2:N$22,N26))</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B27" s="14">
+        <f>1-'S-score-2'!B27/'S-score-2'!B$4</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="14">
+        <f>1-'S-score-2'!C27/'S-score-2'!C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="14">
+        <f>1-'S-score-2'!D27/'S-score-2'!D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="14">
+        <f>1-'S-score-2'!E27/'S-score-2'!E$4</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="14">
+        <f>1-'S-score-2'!F27/'S-score-2'!F$4</f>
+        <v>0.30075187969924799</v>
+      </c>
+      <c r="G27" s="14">
+        <f>1-'S-score-2'!G27/'S-score-2'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="14">
+        <f>1-'S-score-2'!H27/'S-score-2'!H$4</f>
+        <v>1</v>
+      </c>
+      <c r="I27" s="14">
+        <f>1-'S-score-2'!I27/'S-score-2'!I$4</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="14">
+        <f>1-'S-score-2'!J27/'S-score-2'!J$4</f>
+        <v>1</v>
+      </c>
+      <c r="K27" s="14">
+        <f>1-'S-score-2'!K27/'S-score-2'!K$4</f>
+        <v>1</v>
+      </c>
+      <c r="L27" s="14">
+        <f>1-'S-score-2'!L27/'S-score-2'!L$4</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="14">
+        <f>1-'S-score-2'!M27/'S-score-2'!M$4</f>
+        <v>1</v>
+      </c>
+      <c r="N27" s="43">
+        <f t="shared" si="2"/>
+        <v>0.95517640254482361</v>
+      </c>
+      <c r="O27" s="14">
+        <f>RANK(N27,(N$2:N$22,N27))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B28" s="14">
+        <f>1-'S-score-2'!B28/'S-score-2'!B$4</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="14">
+        <f>1-'S-score-2'!C28/'S-score-2'!C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="14">
+        <f>1-'S-score-2'!D28/'S-score-2'!D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="14">
+        <f>1-'S-score-2'!E28/'S-score-2'!E$4</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="14">
+        <f>1-'S-score-2'!F28/'S-score-2'!F$4</f>
+        <v>0.29490392648287389</v>
+      </c>
+      <c r="G28" s="14">
+        <f>1-'S-score-2'!G28/'S-score-2'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="14">
+        <f>1-'S-score-2'!H28/'S-score-2'!H$4</f>
+        <v>0.2993827160493826</v>
+      </c>
+      <c r="I28" s="14">
+        <f>1-'S-score-2'!I28/'S-score-2'!I$4</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="14">
+        <f>1-'S-score-2'!J28/'S-score-2'!J$4</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="14">
+        <f>1-'S-score-2'!K28/'S-score-2'!K$4</f>
+        <v>1</v>
+      </c>
+      <c r="L28" s="14">
+        <f>1-'S-score-2'!L28/'S-score-2'!L$4</f>
+        <v>0.31498279637159832</v>
+      </c>
+      <c r="M28" s="14">
+        <f>1-'S-score-2'!M28/'S-score-2'!M$4</f>
+        <v>1</v>
+      </c>
+      <c r="N28" s="43">
+        <f t="shared" si="2"/>
+        <v>0.79532063339548242</v>
+      </c>
+      <c r="O28" s="14">
+        <f>RANK(N28,(N$2:N$22,N28))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B29" s="14">
+        <f>1-'S-score-2'!B29/'S-score-2'!B$4</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="14">
+        <f>1-'S-score-2'!C29/'S-score-2'!C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="14">
+        <f>1-'S-score-2'!D29/'S-score-2'!D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E29" s="14">
+        <f>1-'S-score-2'!E29/'S-score-2'!E$4</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="14">
+        <f>1-'S-score-2'!F29/'S-score-2'!F$4</f>
+        <v>0.29761904761904756</v>
+      </c>
+      <c r="G29" s="14">
+        <f>1-'S-score-2'!G29/'S-score-2'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="14">
+        <f>1-'S-score-2'!H29/'S-score-2'!H$4</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="14">
+        <f>1-'S-score-2'!I29/'S-score-2'!I$4</f>
+        <v>1</v>
+      </c>
+      <c r="J29" s="14">
+        <f>1-'S-score-2'!J29/'S-score-2'!J$4</f>
+        <v>1</v>
+      </c>
+      <c r="K29" s="14">
+        <f>1-'S-score-2'!K29/'S-score-2'!K$4</f>
+        <v>1</v>
+      </c>
+      <c r="L29" s="14">
+        <f>1-'S-score-2'!L29/'S-score-2'!L$4</f>
+        <v>0.286831404441664</v>
+      </c>
+      <c r="M29" s="14">
+        <f>1-'S-score-2'!M29/'S-score-2'!M$4</f>
+        <v>1</v>
+      </c>
+      <c r="N29" s="43">
+        <f t="shared" si="2"/>
+        <v>0.8544005216276096</v>
+      </c>
+      <c r="O29" s="14">
+        <f>RANK(N29,(N$2:N$22,N29))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B30" s="14">
+        <f>1-'S-score-2'!B30/'S-score-2'!B$4</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="14">
+        <f>1-'S-score-2'!C30/'S-score-2'!C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="14">
+        <f>1-'S-score-2'!D30/'S-score-2'!D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E30" s="14">
+        <f>1-'S-score-2'!E30/'S-score-2'!E$4</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="14">
+        <f>1-'S-score-2'!F30/'S-score-2'!F$4</f>
+        <v>0.30701754385964908</v>
+      </c>
+      <c r="G30" s="14">
+        <f>1-'S-score-2'!G30/'S-score-2'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="14">
+        <f>1-'S-score-2'!H30/'S-score-2'!H$4</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="14">
+        <f>1-'S-score-2'!I30/'S-score-2'!I$4</f>
+        <v>1</v>
+      </c>
+      <c r="J30" s="14">
+        <f>1-'S-score-2'!J30/'S-score-2'!J$4</f>
+        <v>1</v>
+      </c>
+      <c r="K30" s="14">
+        <f>1-'S-score-2'!K30/'S-score-2'!K$4</f>
+        <v>1</v>
+      </c>
+      <c r="L30" s="14">
+        <f>1-'S-score-2'!L30/'S-score-2'!L$4</f>
+        <v>0.28714419768532995</v>
+      </c>
+      <c r="M30" s="14">
+        <f>1-'S-score-2'!M30/'S-score-2'!M$4</f>
+        <v>1</v>
+      </c>
+      <c r="N30" s="43">
+        <f t="shared" si="2"/>
+        <v>0.85504710120303684</v>
+      </c>
+      <c r="O30" s="14">
+        <f>RANK(N30,(N$2:N$22,N30))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" s="14">
+        <f>1-'S-score-2'!B31/'S-score-2'!B$4</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="14">
+        <f>1-'S-score-2'!C31/'S-score-2'!C$4</f>
+        <v>1</v>
+      </c>
+      <c r="D31" s="14">
+        <f>1-'S-score-2'!D31/'S-score-2'!D$4</f>
+        <v>1</v>
+      </c>
+      <c r="E31" s="14">
+        <f>1-'S-score-2'!E31/'S-score-2'!E$4</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="14">
+        <f>1-'S-score-2'!F31/'S-score-2'!F$4</f>
+        <v>1</v>
+      </c>
+      <c r="G31" s="14">
+        <f>1-'S-score-2'!G31/'S-score-2'!G$4</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="14">
+        <f>1-'S-score-2'!H31/'S-score-2'!H$4</f>
+        <v>1</v>
+      </c>
+      <c r="I31" s="14">
+        <f>1-'S-score-2'!I31/'S-score-2'!I$4</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="14">
+        <f>1-'S-score-2'!J31/'S-score-2'!J$4</f>
+        <v>1</v>
+      </c>
+      <c r="K31" s="14">
+        <f>1-'S-score-2'!K31/'S-score-2'!K$4</f>
+        <v>1</v>
+      </c>
+      <c r="L31" s="14">
+        <f>1-'S-score-2'!L31/'S-score-2'!L$4</f>
+        <v>1</v>
+      </c>
+      <c r="M31" s="14">
+        <f>1-'S-score-2'!M31/'S-score-2'!M$4</f>
+        <v>1</v>
+      </c>
+      <c r="N31" s="43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O31" s="14">
+        <f>RANK(N31,(N$2:N$22,N31))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>